<commit_message>
add more details on RIN calculation
</commit_message>
<xml_diff>
--- a/biorefineries/wwt/data/RIN_D3_price.xlsx
+++ b/biorefineries/wwt/data/RIN_D3_price.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yalin\Documents\Coding\Bioindustrial-Park\biorefineries\wwt\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD77DD83-47E1-4C3D-90B5-EB9DA457AF98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A2E36FD-012F-41E6-818C-BEB94711BF27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1360" yWindow="2400" windowWidth="21600" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38430" yWindow="1305" windowWidth="21600" windowHeight="11175" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RIN_D3_price" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
     <author>tc={51D4FABD-9F00-441A-836A-98AE0684D1E7}</author>
   </authors>
   <commentList>
-    <comment ref="M3" authorId="0" shapeId="0" xr:uid="{51D4FABD-9F00-441A-836A-98AE0684D1E7}">
+    <comment ref="L3" authorId="0" shapeId="0" xr:uid="{51D4FABD-9F00-441A-836A-98AE0684D1E7}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1636" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1661" uniqueCount="44">
   <si>
     <t>Transfer Date by Week</t>
   </si>
@@ -132,6 +132,57 @@
   </si>
   <si>
     <t>avg</t>
+  </si>
+  <si>
+    <t>$/gal-to-$/mcf</t>
+  </si>
+  <si>
+    <t>btu</t>
+  </si>
+  <si>
+    <t>MJ=</t>
+  </si>
+  <si>
+    <t>1 kg=</t>
+  </si>
+  <si>
+    <t>1 mcf=</t>
+  </si>
+  <si>
+    <t>scf=</t>
+  </si>
+  <si>
+    <t>mcf</t>
+  </si>
+  <si>
+    <t>LHV of LNG</t>
+  </si>
+  <si>
+    <t>1 btu=</t>
+  </si>
+  <si>
+    <t>MJ</t>
+  </si>
+  <si>
+    <t>MJ/kg=</t>
+  </si>
+  <si>
+    <t>btu/kg</t>
+  </si>
+  <si>
+    <t>LHV of ethanol</t>
+  </si>
+  <si>
+    <t>1 kg LNG=</t>
+  </si>
+  <si>
+    <t>gal ethanol</t>
+  </si>
+  <si>
+    <t>1 mcf LNG=</t>
+  </si>
+  <si>
+    <t>btu/gal</t>
   </si>
 </sst>
 </file>
@@ -459,7 +510,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -654,6 +705,43 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -699,7 +787,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -709,11 +797,31 @@
     <xf numFmtId="8" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="16" xfId="6" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1067,7 +1175,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1075,7 +1183,7 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="M3" dT="2023-01-28T19:25:56.05" personId="{584F5FDF-96FF-4D00-8D77-0B152281502D}" id="{51D4FABD-9F00-441A-836A-98AE0684D1E7}">
+  <threadedComment ref="L3" dT="2023-01-28T19:25:56.05" personId="{584F5FDF-96FF-4D00-8D77-0B152281502D}" id="{51D4FABD-9F00-441A-836A-98AE0684D1E7}">
     <text>0.599 gal/kg*1/0.04544 kg/mcf</text>
   </threadedComment>
 </ThreadedComments>
@@ -1083,15 +1191,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N807"/>
+  <dimension ref="A1:T807"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K227" sqref="K227"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="7" max="7" width="10.58203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.83203125" style="13" customWidth="1"/>
+    <col min="16" max="16" width="12.75" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1113,7 +1226,7 @@
       <c r="G1" t="s">
         <v>8</v>
       </c>
-      <c r="H1">
+      <c r="H1" s="13">
         <f>AVERAGE(F:F)</f>
         <v>1.8429900744416856</v>
       </c>
@@ -1121,7 +1234,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>42009</v>
       </c>
@@ -1143,14 +1256,14 @@
       <c r="G2" s="3">
         <v>-0.25</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="13">
         <v>1.382242556</v>
       </c>
       <c r="J2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>42030</v>
       </c>
@@ -1172,7 +1285,7 @@
       <c r="G3" s="3">
         <v>0.25</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="13">
         <v>2.3037375930000001</v>
       </c>
       <c r="K3" t="s">
@@ -1182,10 +1295,24 @@
         <v>22</v>
       </c>
       <c r="M3" t="s">
+        <v>22</v>
+      </c>
+      <c r="N3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="P3" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q3" s="29"/>
+      <c r="R3" s="30"/>
+      <c r="S3" s="30">
+        <v>77000</v>
+      </c>
+      <c r="T3" s="31" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>42051</v>
       </c>
@@ -1212,18 +1339,38 @@
         <v>0.90329268292682918</v>
       </c>
       <c r="L4" s="2">
+        <f>K4*$S$13</f>
+        <v>11.531645549572378</v>
+      </c>
+      <c r="M4" s="2">
         <v>4.26</v>
       </c>
-      <c r="M4" s="2">
-        <f>K4*0.599*1/0.04544</f>
-        <v>11.907401344039846</v>
-      </c>
-      <c r="N4" s="4">
-        <f>M4/L4</f>
-        <v>2.7951646347511376</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="N4" s="2">
+        <f>M4/$S$13</f>
+        <v>0.33369277721261442</v>
+      </c>
+      <c r="O4" s="4">
+        <f>L4/M4</f>
+        <v>2.7069590491953939</v>
+      </c>
+      <c r="P4" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q4" s="15">
+        <v>47.13</v>
+      </c>
+      <c r="R4" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="S4" s="15">
+        <f>Q4*947</f>
+        <v>44632.11</v>
+      </c>
+      <c r="T4" s="17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>42058</v>
       </c>
@@ -1245,7 +1392,7 @@
       <c r="G5" t="s">
         <v>9</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="13">
         <f>_xlfn.PERCENTILE.INC(F:F, 0)</f>
         <v>0.46</v>
       </c>
@@ -1257,18 +1404,38 @@
         <v>1.5460839160839162</v>
       </c>
       <c r="L5" s="2">
+        <f>K5*$S$13</f>
+        <v>19.737668694941423</v>
+      </c>
+      <c r="M5" s="2">
         <v>3.71</v>
       </c>
-      <c r="M5" s="2">
-        <f t="shared" ref="M5:M10" si="0">K5*0.599*1/0.04544</f>
-        <v>20.380815707180144</v>
-      </c>
-      <c r="N5" s="4">
-        <f t="shared" ref="N5:N10" si="1">M5/L5</f>
-        <v>5.4934813226900658</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="N5" s="2">
+        <f>M5/$S$13</f>
+        <v>0.29061037639877924</v>
+      </c>
+      <c r="O5" s="4">
+        <f>L5/M5</f>
+        <v>5.3201263328683082</v>
+      </c>
+      <c r="P5" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q5" s="19">
+        <v>1000</v>
+      </c>
+      <c r="R5" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="S5" s="20">
+        <f>983*1000</f>
+        <v>983000</v>
+      </c>
+      <c r="T5" s="21" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>42065</v>
       </c>
@@ -1290,7 +1457,7 @@
       <c r="G6" t="s">
         <v>10</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="13">
         <f>_xlfn.PERCENTILE.INC(F:F, 0.05)</f>
         <v>0.77</v>
       </c>
@@ -1302,18 +1469,34 @@
         <v>2.4574782608695638</v>
       </c>
       <c r="L6" s="2">
+        <f>K6*$S$13</f>
+        <v>31.372741953698455</v>
+      </c>
+      <c r="M6" s="2">
         <v>4.16</v>
       </c>
-      <c r="M6" s="2">
-        <f t="shared" si="0"/>
-        <v>32.395014926515593</v>
-      </c>
-      <c r="N6" s="4">
-        <f t="shared" si="1"/>
-        <v>7.7872632034893252</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="N6" s="2">
+        <f>M6/$S$13</f>
+        <v>0.32585961342828079</v>
+      </c>
+      <c r="O6" s="4">
+        <f>L6/M6</f>
+        <v>7.5415245081005899</v>
+      </c>
+      <c r="P6" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q6" s="20">
+        <f>S4/S5</f>
+        <v>4.5403977619532049E-2</v>
+      </c>
+      <c r="R6" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="S6" s="20"/>
+      <c r="T6" s="21"/>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>42065</v>
       </c>
@@ -1335,7 +1518,7 @@
       <c r="G7" t="s">
         <v>11</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="13">
         <f>_xlfn.PERCENTILE.INC(F:F, 0.1)</f>
         <v>0.89500000000000002</v>
       </c>
@@ -1347,18 +1530,32 @@
         <v>2.3452586206896546</v>
       </c>
       <c r="L7" s="2">
+        <f>K7*$S$13</f>
+        <v>29.940119793999095</v>
+      </c>
+      <c r="M7" s="2">
         <v>4.2300000000000004</v>
       </c>
-      <c r="M7" s="2">
-        <f t="shared" si="0"/>
-        <v>30.915711131010191</v>
-      </c>
-      <c r="N7" s="4">
-        <f t="shared" si="1"/>
-        <v>7.3086787543759311</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="N7" s="2">
+        <f>M7/$S$13</f>
+        <v>0.33134282807731441</v>
+      </c>
+      <c r="O7" s="4">
+        <f>L7/M7</f>
+        <v>7.0780425044915107</v>
+      </c>
+      <c r="P7" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q7" s="25">
+        <f>0.599*1/Q6</f>
+        <v>13.192676752230623</v>
+      </c>
+      <c r="R7" s="26"/>
+      <c r="S7" s="26"/>
+      <c r="T7" s="27"/>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>42065</v>
       </c>
@@ -1380,7 +1577,7 @@
       <c r="G8" t="s">
         <v>12</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="13">
         <f>_xlfn.PERCENTILE.INC(F:F, 0.25)</f>
         <v>1.25</v>
       </c>
@@ -1392,18 +1589,33 @@
         <v>1.3361458333333334</v>
       </c>
       <c r="L8" s="2">
+        <f>K8*$S$13</f>
+        <v>17.057550054112554</v>
+      </c>
+      <c r="M8" s="2">
         <v>3.81</v>
       </c>
-      <c r="M8" s="2">
-        <f t="shared" si="0"/>
-        <v>17.613366068808684</v>
-      </c>
-      <c r="N8" s="4">
-        <f t="shared" si="1"/>
-        <v>4.6229307267214397</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="N8" s="2">
+        <f>M8/$S$13</f>
+        <v>0.29844354018311292</v>
+      </c>
+      <c r="O8" s="4">
+        <f>L8/M8</f>
+        <v>4.477047258297258</v>
+      </c>
+      <c r="P8" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q8" s="22">
+        <v>1.0549999999999999E-3</v>
+      </c>
+      <c r="R8" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="S8" s="20"/>
+      <c r="T8" s="21"/>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>42072</v>
       </c>
@@ -1425,7 +1637,7 @@
       <c r="G9" t="s">
         <v>14</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="13">
         <f>_xlfn.PERCENTILE.INC(F:F, 0.5)</f>
         <v>1.8</v>
       </c>
@@ -1437,18 +1649,38 @@
         <v>1.3196799999999997</v>
       </c>
       <c r="L9" s="2">
+        <f>K9*$S$13</f>
+        <v>16.847343376623375</v>
+      </c>
+      <c r="M9" s="2">
         <v>3.43</v>
       </c>
-      <c r="M9" s="2">
-        <f t="shared" si="0"/>
-        <v>17.396309859154925</v>
-      </c>
-      <c r="N9" s="4">
-        <f t="shared" si="1"/>
-        <v>5.0718104545641181</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="N9" s="2">
+        <f>M9/$S$13</f>
+        <v>0.26867751780264498</v>
+      </c>
+      <c r="O9" s="4">
+        <f>L9/M9</f>
+        <v>4.9117619173829077</v>
+      </c>
+      <c r="P9" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q9" s="23">
+        <v>48.62</v>
+      </c>
+      <c r="R9" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="S9" s="20">
+        <f>Q9/Q8</f>
+        <v>46085.30805687204</v>
+      </c>
+      <c r="T9" s="21" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>42072</v>
       </c>
@@ -1470,7 +1702,7 @@
       <c r="G10" t="s">
         <v>15</v>
       </c>
-      <c r="H10">
+      <c r="H10" s="13">
         <f>_xlfn.PERCENTILE.INC(F:F, 0.75)</f>
         <v>2.4500000000000002</v>
       </c>
@@ -1482,18 +1714,34 @@
         <v>2.6542635658914735</v>
       </c>
       <c r="L10" s="2">
+        <f>K10*$S$13</f>
+        <v>33.884949159367771</v>
+      </c>
+      <c r="M10" s="2">
         <v>6.02</v>
       </c>
-      <c r="M10" s="2">
-        <f t="shared" si="0"/>
-        <v>34.989081777486632</v>
-      </c>
-      <c r="N10" s="4">
-        <f t="shared" si="1"/>
-        <v>5.8121398301472817</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="N10" s="2">
+        <f>M10/$S$13</f>
+        <v>0.47155645981688704</v>
+      </c>
+      <c r="O10" s="4">
+        <f>L10/M10</f>
+        <v>5.6287290962404937</v>
+      </c>
+      <c r="P10" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q10" s="24"/>
+      <c r="R10" s="20"/>
+      <c r="S10" s="20">
+        <f>S9/S3</f>
+        <v>0.5985104942450914</v>
+      </c>
+      <c r="T10" s="21" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>42086</v>
       </c>
@@ -1515,7 +1763,7 @@
       <c r="G11" t="s">
         <v>16</v>
       </c>
-      <c r="H11">
+      <c r="H11" s="13">
         <f>_xlfn.PERCENTILE.INC(F:F, 0.9)</f>
         <v>2.77</v>
       </c>
@@ -1527,19 +1775,33 @@
         <v>1.7946004113992531</v>
       </c>
       <c r="L11" s="6">
-        <f t="shared" ref="L11:N11" si="2">AVERAGE(L4:L10)</f>
+        <f>AVERAGE(L4:L10)</f>
+        <v>22.910288368902147</v>
+      </c>
+      <c r="M11" s="6">
+        <f t="shared" ref="M11:O11" si="0">AVERAGE(M4:M10)</f>
         <v>4.2314285714285713</v>
       </c>
-      <c r="M11" s="6">
-        <f t="shared" si="2"/>
-        <v>23.656814402028004</v>
-      </c>
-      <c r="N11" s="7">
-        <f t="shared" si="2"/>
-        <v>5.5559241323913282</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="N11" s="6">
+        <f t="shared" ref="N11" si="1">AVERAGE(N4:N10)</f>
+        <v>0.33145473041709056</v>
+      </c>
+      <c r="O11" s="7">
+        <f t="shared" si="0"/>
+        <v>5.3805986666537802</v>
+      </c>
+      <c r="P11" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q11" s="25">
+        <f>0.599*1/(S9/S5)</f>
+        <v>12.776674928013161</v>
+      </c>
+      <c r="R11" s="26"/>
+      <c r="S11" s="26"/>
+      <c r="T11" s="27"/>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>42086</v>
       </c>
@@ -1561,31 +1823,51 @@
       <c r="G12" t="s">
         <v>17</v>
       </c>
-      <c r="H12">
+      <c r="H12" s="13">
         <f>_xlfn.PERCENTILE.INC(F:F, 0.95)</f>
         <v>2.95</v>
       </c>
       <c r="J12" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="K12" s="9">
+      <c r="K12" s="2">
         <f>MIN(K4:K10)</f>
         <v>0.90329268292682918</v>
       </c>
-      <c r="L12" s="9">
+      <c r="L12" s="2">
         <f>MIN(L4:L10)</f>
+        <v>11.531645549572378</v>
+      </c>
+      <c r="M12" s="2">
+        <f>MIN(M4:M10)</f>
         <v>3.43</v>
       </c>
-      <c r="M12" s="9">
-        <f>MIN(M4:M10)</f>
-        <v>11.907401344039846</v>
-      </c>
-      <c r="N12" s="10">
+      <c r="N12" s="2">
         <f>MIN(N4:N10)</f>
-        <v>2.7951646347511376</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+        <v>0.26867751780264498</v>
+      </c>
+      <c r="O12" s="9">
+        <f>MIN(O4:O10)</f>
+        <v>2.7069590491953939</v>
+      </c>
+      <c r="P12" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q12" s="15">
+        <v>1000</v>
+      </c>
+      <c r="R12" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="S12" s="16">
+        <f>983*1000</f>
+        <v>983000</v>
+      </c>
+      <c r="T12" s="17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>42093</v>
       </c>
@@ -1607,31 +1889,47 @@
       <c r="G13" t="s">
         <v>18</v>
       </c>
-      <c r="H13">
+      <c r="H13" s="13">
         <f>_xlfn.PERCENTILE.INC(F:F, 1)</f>
         <v>3.46</v>
       </c>
-      <c r="J13" s="11" t="s">
+      <c r="J13" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="K13" s="12">
+      <c r="K13" s="11">
         <f>MAX(K4:K10)</f>
         <v>2.6542635658914735</v>
       </c>
-      <c r="L13" s="12">
+      <c r="L13" s="11">
         <f>MAX(L4:L10)</f>
+        <v>33.884949159367771</v>
+      </c>
+      <c r="M13" s="11">
+        <f>MAX(M4:M10)</f>
         <v>6.02</v>
       </c>
-      <c r="M13" s="12">
-        <f>MAX(M4:M10)</f>
-        <v>34.989081777486632</v>
-      </c>
-      <c r="N13" s="13">
+      <c r="N13" s="11">
         <f>MAX(N4:N10)</f>
-        <v>7.7872632034893252</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
+        <v>0.47155645981688704</v>
+      </c>
+      <c r="O13" s="12">
+        <f>MAX(O4:O10)</f>
+        <v>7.5415245081005899</v>
+      </c>
+      <c r="P13" s="32" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q13" s="11"/>
+      <c r="R13" s="26"/>
+      <c r="S13" s="33">
+        <f>S12/S3</f>
+        <v>12.766233766233766</v>
+      </c>
+      <c r="T13" s="27" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>42093</v>
       </c>
@@ -1653,7 +1951,7 @@
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
     </row>
-    <row r="15" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>42100</v>
       </c>
@@ -1675,7 +1973,7 @@
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
     </row>
-    <row r="16" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>42107</v>
       </c>
@@ -6315,7 +6613,7 @@
         <v>2.4</v>
       </c>
       <c r="K226" s="2"/>
-      <c r="L226" s="2"/>
+      <c r="L226" s="13"/>
     </row>
     <row r="227" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A227" s="1">
@@ -6337,7 +6635,7 @@
         <v>2.17</v>
       </c>
       <c r="K227" s="2"/>
-      <c r="L227" s="2"/>
+      <c r="L227" s="13"/>
     </row>
     <row r="228" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A228" s="1">
@@ -8844,8 +9142,6 @@
       <c r="F341" s="2">
         <v>2.69</v>
       </c>
-      <c r="K341" s="2"/>
-      <c r="L341" s="2"/>
     </row>
     <row r="342" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A342" s="1">
@@ -8866,8 +9162,6 @@
       <c r="F342" s="2">
         <v>2.8</v>
       </c>
-      <c r="K342" s="2"/>
-      <c r="L342" s="2"/>
     </row>
     <row r="343" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A343" s="1">
@@ -11396,8 +11690,6 @@
       <c r="F457" s="2">
         <v>2.2999999999999998</v>
       </c>
-      <c r="K457" s="2"/>
-      <c r="L457" s="2"/>
     </row>
     <row r="458" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A458" s="1">
@@ -13508,8 +13800,6 @@
       <c r="F553" s="2">
         <v>0.8</v>
       </c>
-      <c r="K553" s="2"/>
-      <c r="L553" s="2"/>
     </row>
     <row r="554" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A554" s="1">
@@ -13530,8 +13820,6 @@
       <c r="F554" s="2">
         <v>0.81</v>
       </c>
-      <c r="K554" s="2"/>
-      <c r="L554" s="2"/>
     </row>
     <row r="555" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A555" s="1">
@@ -16258,8 +16546,6 @@
       <c r="F678" s="2">
         <v>1.94</v>
       </c>
-      <c r="K678" s="2"/>
-      <c r="L678" s="2"/>
     </row>
     <row r="679" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A679" s="1">
@@ -16280,8 +16566,6 @@
       <c r="F679" s="2">
         <v>1.92</v>
       </c>
-      <c r="K679" s="2"/>
-      <c r="L679" s="2"/>
     </row>
     <row r="680" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A680" s="1">

</xml_diff>